<commit_message>
New features, new class
- Added le_Engine diagnostics for real-time CPU utilization debugging and information. Also added, le_Element CPU engine utilization.
- renamed python test file for le_Analog1PWinding
- added le_Config.h
- Added le_UARTTx class for general print buffer management.
- le_IRIGB is fixed, unmanaged increment was overwriting adjacent data. Fixed.
</commit_message>
<xml_diff>
--- a/tests/le_Update_Times.xlsx
+++ b/tests/le_Update_Times.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8210f83787c5f981/Documents/GitHub/LogicElements/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="145" documentId="8_{667BEF11-9D92-47ED-8245-FD9A9C149588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B46CF98-3418-4274-B6C9-0E7D3CFB3DE6}"/>
+  <xr:revisionPtr revIDLastSave="153" documentId="8_{667BEF11-9D92-47ED-8245-FD9A9C149588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAECE266-947F-48BA-ADE1-63D98B2A0A69}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="3495" windowWidth="34170" windowHeight="15435" xr2:uid="{B699E6CA-9989-4110-B8DD-DB05DC3280B6}"/>
+    <workbookView xWindow="15840" yWindow="2205" windowWidth="34170" windowHeight="15435" activeTab="1" xr2:uid="{B699E6CA-9989-4110-B8DD-DB05DC3280B6}"/>
   </bookViews>
   <sheets>
     <sheet name="STM32F4" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">STM32F4!$A$4:$E$4</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
   <si>
     <t>Function</t>
   </si>
@@ -129,6 +130,15 @@
   </si>
   <si>
     <t>2x1</t>
+  </si>
+  <si>
+    <t>le_Time::Decode()</t>
+  </si>
+  <si>
+    <t>8 frames</t>
+  </si>
+  <si>
+    <t>exc_time = 45.6 us (max)</t>
   </si>
 </sst>
 </file>
@@ -546,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC3FAC2-DBE1-4835-A3F6-1DB5517F72FB}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,7 +892,7 @@
         <v>0.1176</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" ref="E19:E20" si="5">ROUNDUP($B$2*1000000/C19*D19, 0)</f>
+        <f t="shared" ref="E19" si="5">ROUNDUP($B$2*1000000/C19*D19, 0)</f>
         <v>2573</v>
       </c>
       <c r="F19" s="1" t="s">
@@ -972,7 +982,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="E24" s="1">
-        <f t="shared" ref="E24:E25" si="9">ROUNDUP($B$2*1000000/C24*D24, 0)</f>
+        <f t="shared" ref="E24" si="9">ROUNDUP($B$2*1000000/C24*D24, 0)</f>
         <v>175</v>
       </c>
     </row>
@@ -1040,6 +1050,20 @@
       <c r="E28" s="1">
         <f t="shared" ref="E28" si="12">ROUNDUP($B$2*1000000/C28*D28, 0)</f>
         <v>302</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="1">
+        <v>3830</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1051,4 +1075,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E087AC9-3385-4613-9502-6FD31CAA1344}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>